<commit_message>
Implementación de busqueda por nombre y sección
</commit_message>
<xml_diff>
--- a/EasyWay-Backend/inventarioBackend/productos.xlsx
+++ b/EasyWay-Backend/inventarioBackend/productos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>Electrónica</t>
+  </si>
+  <si>
+    <t>Play Station 5</t>
+  </si>
+  <si>
+    <t>Martillo</t>
+  </si>
+  <si>
+    <t>Ferretería</t>
   </si>
 </sst>
 </file>
@@ -77,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,6 +126,40 @@
         <v>1500.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>1000.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>1000.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>1500.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización Frontend con funciones de busqueda
</commit_message>
<xml_diff>
--- a/EasyWay-Backend/inventarioBackend/productos.xlsx
+++ b/EasyWay-Backend/inventarioBackend/productos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -35,13 +35,19 @@
     <t>Electrónica</t>
   </si>
   <si>
-    <t>Play Station 5</t>
+    <t xml:space="preserve">Computador </t>
   </si>
   <si>
-    <t>Martillo</t>
+    <t>Tecnología</t>
   </si>
   <si>
-    <t>Ferretería</t>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>Comedor 4 Puestos</t>
+  </si>
+  <si>
+    <t>Hogar</t>
   </si>
 </sst>
 </file>
@@ -86,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -128,36 +134,53 @@
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>1000.0</v>
+        <v>300000.0</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>1500.0</v>
+        <v>500000.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>3.0</v>
+        <v>9.0</v>
       </c>
       <c r="B4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>9</v>
-      </c>
       <c r="D4" t="n" s="0">
-        <v>1000.0</v>
+        <v>4000000.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>1500.0</v>
+        <v>7000000.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>250000.0</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>300000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementación de busqueda en archivo de indice manual
</commit_message>
<xml_diff>
--- a/EasyWay-Backend/inventarioBackend/productos.xlsx
+++ b/EasyWay-Backend/inventarioBackend/productos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -42,6 +42,36 @@
   </si>
   <si>
     <t>Ferretería</t>
+  </si>
+  <si>
+    <t>Televisor LG</t>
+  </si>
+  <si>
+    <t>Televisor Samsung</t>
+  </si>
+  <si>
+    <t>Set vasos x 6 UND</t>
+  </si>
+  <si>
+    <t>Hogar</t>
+  </si>
+  <si>
+    <t>Silla Rimax</t>
+  </si>
+  <si>
+    <t>Manzana</t>
+  </si>
+  <si>
+    <t>Alimentos</t>
+  </si>
+  <si>
+    <t>Granadilla</t>
+  </si>
+  <si>
+    <t>Camiseta Nike</t>
+  </si>
+  <si>
+    <t>Ropa</t>
   </si>
 </sst>
 </file>
@@ -86,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -160,6 +190,125 @@
         <v>1500.0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>1000.0</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>1000.0</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>1000.0</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>1000.0</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>1000.0</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>1000.0</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D11" t="n" s="0">
+        <v>1000.0</v>
+      </c>
+      <c r="E11" t="n" s="0">
+        <v>1500.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>